<commit_message>
Stopped scatter plot from taking focus during run
</commit_message>
<xml_diff>
--- a/SetupAB.xlsx
+++ b/SetupAB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotab\Documents\GitHub\Auto-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007070DE-0877-4167-A4DF-D80CE185E7D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016A7B4B-D413-4F04-912D-2AD983766D7F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18340" windowHeight="12030" tabRatio="522" activeTab="1" xr2:uid="{3886B5EF-EF21-4DBC-AA87-02E9D999E081}"/>
   </bookViews>
@@ -612,7 +612,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CF5EA2B-B917-4EC7-B055-2E3E6648F473}" type="CELLRANGE">
+                    <a:fld id="{80C704CD-DD66-4EB1-B878-4A672C77B2B0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -644,8 +644,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C8E5BAC3-741D-4148-AC00-3C47C0E64EA1}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{A07F60A9-EAD4-44B0-8535-BC07E6E1ECCD}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -662,6 +662,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -676,8 +677,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AD90D460-0C08-4130-B2CA-B8D619FD97B3}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{73807196-7C31-4394-AAD5-D5C017434B51}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -694,6 +695,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -708,8 +710,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5582E58B-9113-4064-BC6E-D7BE2673D6E2}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{EDE667C1-514F-44DF-B9EA-4297178C3B22}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -726,6 +728,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -740,8 +743,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{807B7005-90AD-44D8-BFB5-908603584010}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{1CAA2BE3-DA98-493E-96DF-421FDD800F26}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -758,6 +761,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -772,8 +776,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{51962BA2-4220-4740-8E7C-17E9378C1449}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{28EE4E67-87B0-4083-891F-1C54A78B8131}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -790,6 +794,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -804,8 +809,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07A782E8-54E8-4C63-8C77-CEB35AD5AC77}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{1BB8DC5F-AAD3-4CE5-AFFF-E53B1588BFF1}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -822,6 +827,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -836,8 +842,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5299D73A-74D5-4712-A1AD-753AB7B87F1F}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{E9935845-27C8-4031-9AFE-324E6AACA6D6}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -854,6 +860,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -868,8 +875,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E15B44F5-EBF8-4A99-B66A-F3494144266B}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{31CD2C71-D5AD-40CA-9B9B-A0CFD1EDBF50}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -886,6 +893,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -900,8 +908,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{756A5100-1069-422C-9148-CA42E3795BA7}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{0E7CBE27-8BEA-4ED1-9448-2849FC32C5E5}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -918,6 +926,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -932,8 +941,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{12CFAC3C-171F-403A-885B-686AA1FB6887}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{B54496A3-C1A6-472E-966D-1CEC05C904BE}" type="CELLRANGE">
+                      <a:rPr lang="en-CA"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -950,6 +959,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2255,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7214811-FEDE-4101-9CF3-2833DAA480B0}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2553,8 +2563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B8BD7A-1168-4EE3-A8DD-8254CC158A6A}">
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4451,7 +4461,7 @@
   <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4851,7 +4861,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5197,7 +5207,7 @@
   <dimension ref="A1:AM23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Finished Rectangular Columns Function
</commit_message>
<xml_diff>
--- a/SetupAB.xlsx
+++ b/SetupAB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kotab\Documents\GitHub\Auto-Builder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexv\Documents\GitHub\Auto-Builder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB66B05-5CA2-43C9-B6B2-D3D573BC4365}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104F88F8-5813-47BD-AB06-716EED0124DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18340" windowHeight="12030" tabRatio="522" xr2:uid="{3886B5EF-EF21-4DBC-AA87-02E9D999E081}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="522" xr2:uid="{3886B5EF-EF21-4DBC-AA87-02E9D999E081}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="4" r:id="rId1"/>
@@ -384,15 +384,9 @@
     <t>Results location</t>
   </si>
   <si>
-    <t>C:\Users\kotab\OneDrive - University of Toronto\Auto-builder</t>
-  </si>
-  <si>
     <t>Time history location</t>
   </si>
   <si>
-    <t>C:\Users\kotab\OneDrive - University of Toronto\Auto-builder\GM1.txt</t>
-  </si>
-  <si>
     <t>Side 1</t>
   </si>
   <si>
@@ -403,6 +397,12 @@
   </si>
   <si>
     <t>Side 4</t>
+  </si>
+  <si>
+    <t>C:\Users\alexv\Downloads\GM1.txt</t>
+  </si>
+  <si>
+    <t>C:\Users\alexv\Documents\UofT\Auto Builder</t>
   </si>
 </sst>
 </file>
@@ -629,7 +629,7 @@
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -656,12 +656,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5165FB11-5052-4AB8-BD11-C8096E30DC13}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{7DC41E34-FCC0-4C54-9E14-145F6E7DE1DB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -689,12 +689,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ADC2921E-BCF4-4AE1-A905-260D6E4ED770}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{35E38176-1EF5-4C56-B196-F20ED35FEE26}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -722,12 +722,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0B98D51-A611-43FC-949E-249AB4498E05}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{AB083A80-879B-42AB-AE12-EBED651133F4}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -755,12 +755,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{878A18F7-6DF7-4352-8C95-A7C05433F99F}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{3F9A438C-6F35-499F-8833-6BDB9E367ECF}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -788,12 +788,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D70987B6-D322-463C-9F08-530356E1A016}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{E6BEDD81-9B89-4CC3-BC44-E19832A40681}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -821,12 +821,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{429285FE-7680-47E9-ACCB-DAD064B9ED12}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{5CA775CB-4251-4B9C-979C-3B863A137C9F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -854,12 +854,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{07D0604D-59A1-46B6-98C3-47068839C145}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{F9D2C2F6-3C41-46A7-A244-6C1400850CF6}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -887,12 +887,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59ADA7E3-6B51-4FE3-AC4E-ACCBD7A830BB}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{2D39BEC4-DF47-4926-B50F-99A9C55514DB}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -920,12 +920,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC509415-1813-498E-8921-28147CCF8EC9}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{042156B3-CB94-4BEC-929D-3E96309EF09F}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -953,12 +953,12 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B4EDE4B9-5BE6-4F0D-B088-47F667776202}" type="CELLRANGE">
-                      <a:rPr lang="en-CA"/>
+                    <a:fld id="{220AB91F-08CD-408A-A76A-70B8DE217C13}" type="CELLRANGE">
+                      <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
-                    <a:endParaRPr lang="en-CA"/>
+                    <a:endParaRPr lang="en-US"/>
                   </a:p>
                 </c:rich>
               </c:tx>
@@ -2278,16 +2278,16 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>38</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -2319,7 +2319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>49</v>
       </c>
@@ -2351,7 +2351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -2379,7 +2379,7 @@
       </c>
       <c r="C11" s="19"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="C12" s="19"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>66</v>
       </c>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="C13" s="19"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="C14" s="19"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>70</v>
       </c>
@@ -2415,7 +2415,7 @@
       </c>
       <c r="C15" s="19"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -2424,7 +2424,7 @@
       </c>
       <c r="C16" s="19"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -2433,7 +2433,7 @@
       </c>
       <c r="C17" s="19"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -2442,7 +2442,7 @@
       </c>
       <c r="C18" s="19"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>78</v>
       </c>
@@ -2451,7 +2451,7 @@
       </c>
       <c r="C19" s="19"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -2459,7 +2459,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>81</v>
       </c>
@@ -2467,7 +2467,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>87</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -2491,7 +2491,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>90</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>91</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>93</v>
       </c>
@@ -2523,7 +2523,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>94</v>
       </c>
@@ -2531,7 +2531,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -2539,57 +2539,57 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>98</v>
       </c>
       <c r="B32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>101</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>103</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>104</v>
       </c>
       <c r="B35">
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B36">
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -2607,24 +2607,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65B8BD7A-1168-4EE3-A8DD-8254CC158A6A}">
   <dimension ref="A1:X69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="8.7265625" customWidth="1"/>
-    <col min="12" max="12" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>37</v>
       </c>
@@ -2633,7 +2633,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -2669,7 +2669,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2792,7 +2792,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -2834,7 +2834,7 @@
       </c>
       <c r="X9" s="5"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -2876,7 +2876,7 @@
       </c>
       <c r="X10" s="5"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
@@ -2918,11 +2918,11 @@
       </c>
       <c r="X11" s="5"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12" s="8"/>
       <c r="X12" s="5"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>37</v>
       </c>
@@ -2932,7 +2932,7 @@
       <c r="C13" s="2"/>
       <c r="X13" s="5"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="X14" s="5"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -2968,7 +2968,7 @@
       <c r="L17" s="8"/>
       <c r="M17" s="8"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>21</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -3050,7 +3050,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3091,7 +3091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>3</v>
       </c>
@@ -3132,7 +3132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3173,7 +3173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>5</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -3255,7 +3255,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8</v>
       </c>
@@ -3337,7 +3337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -3419,7 +3419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>37</v>
       </c>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -3545,7 +3545,7 @@
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>21</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1</v>
       </c>
@@ -3627,7 +3627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -3791,7 +3791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>37</v>
       </c>
@@ -3800,7 +3800,7 @@
       </c>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -3808,7 +3808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
@@ -3835,7 +3835,7 @@
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>21</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>5</v>
       </c>
@@ -4081,7 +4081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>6</v>
       </c>
@@ -4122,7 +4122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>8</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>37</v>
       </c>
@@ -4213,7 +4213,7 @@
       </c>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
       <c r="C63" s="5"/>
@@ -4248,7 +4248,7 @@
       <c r="L63" s="8"/>
       <c r="M63" s="8"/>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>21</v>
       </c>
@@ -4289,7 +4289,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1</v>
       </c>
@@ -4330,7 +4330,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -4371,7 +4371,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>3</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>4</v>
       </c>
@@ -4453,7 +4453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>5</v>
       </c>
@@ -4508,17 +4508,17 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>24</v>
       </c>
@@ -4544,7 +4544,7 @@
       <c r="P1" s="7"/>
       <c r="Q1" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>26</v>
       </c>
@@ -4594,7 +4594,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4694,7 +4694,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4744,7 +4744,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="18">
         <v>5</v>
       </c>
@@ -4844,7 +4844,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>6</v>
       </c>
@@ -4908,16 +4908,16 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>27</v>
       </c>
@@ -4937,8 +4937,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>0.1963</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -5020,7 +5020,7 @@
         <v>6.136E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -5040,7 +5040,7 @@
         <v>3.068E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>3.068E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>0.1767</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -5100,7 +5100,7 @@
         <v>0.1767</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -5120,7 +5120,7 @@
         <v>1.23E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>1.23E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>2.0799999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5180,7 +5180,7 @@
         <v>2.0799999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -5220,7 +5220,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -5254,9 +5254,9 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -5313,7 +5313,7 @@
       <c r="AL1" s="2"/>
       <c r="AM1" s="2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5527,7 +5527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5907,7 +5907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -6025,7 +6025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -6131,7 +6131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -6178,7 +6178,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="5:37" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:37" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>36</v>
       </c>
@@ -6255,9 +6255,9 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -6314,7 +6314,7 @@
       <c r="AL1" s="2"/>
       <c r="AM1" s="2"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>26</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -6528,7 +6528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -6635,7 +6635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -6742,7 +6742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -6849,7 +6849,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -7026,7 +7026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -7179,7 +7179,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="5:37" x14ac:dyDescent="0.35">
+    <row r="23" spans="5:37" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>36</v>
       </c>
@@ -7257,14 +7257,14 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -7278,8 +7278,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -7307,7 +7307,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -7321,7 +7321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>86</v>
       </c>
@@ -7335,7 +7335,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>200000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -7363,7 +7363,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -7377,23 +7377,23 @@
         <v>117000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>

</xml_diff>